<commit_message>
fix divi corona report
</commit_message>
<xml_diff>
--- a/data/kbvreport_export/faktenblatttabellen_2021-11-28.xlsx
+++ b/data/kbvreport_export/faktenblatttabellen_2021-11-28.xlsx
@@ -771,41 +771,41 @@
     <t xml:space="preserve">Intensivbetten gesamt</t>
   </si>
   <si>
-    <t xml:space="preserve">22180</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22149</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0,1 %</t>
+    <t xml:space="preserve">21908</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21771</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0,6 %</t>
   </si>
   <si>
     <t xml:space="preserve">Belegung durch Patient*innen mit COVID-19</t>
   </si>
   <si>
-    <t xml:space="preserve">3510
-16 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4326
-20 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23,2 %</t>
+    <t xml:space="preserve">3678
+17 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4478
+21 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21,8 %</t>
   </si>
   <si>
     <t xml:space="preserve">Freie Intensivbetten</t>
   </si>
   <si>
-    <t xml:space="preserve">2457
-11 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2277
-10 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-7,3 %</t>
+    <t xml:space="preserve">2776
+13 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2568
+12 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-7,5 %</t>
   </si>
   <si>
     <t xml:space="preserve">Todesfälle &amp; Sterblichkeit</t>

</xml_diff>